<commit_message>
too much work to look fully into. Mainly spatial statistics for single crystals, polycrystals for stiffness, strength and fatigue resistance
</commit_message>
<xml_diff>
--- a/fip_collab/2016_05_18_single_crystal_linkage/npc_npoly.xlsx
+++ b/fip_collab/2016_05_18_single_crystal_linkage/npc_npoly.xlsx
@@ -374,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,39 +404,39 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D2">
         <v>4</v>
       </c>
       <c r="E2">
-        <v>3.4969999999999999</v>
+        <v>2.6100000000000002E-2</v>
       </c>
       <c r="F2">
-        <v>14.363</v>
+        <v>0.126</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
         <v>9</v>
       </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
       <c r="C3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3">
-        <v>0.21</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="F3">
         <v>0.34699999999999998</v>
@@ -444,39 +444,22 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>23</v>
       </c>
       <c r="C4">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4">
-        <v>1324.2260000000001</v>
+        <v>177.53800000000001</v>
       </c>
       <c r="F4">
-        <v>2132.9670000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>23</v>
-      </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>2607.3719999999998</v>
-      </c>
-      <c r="F5">
-        <v>9461.8089999999993</v>
+        <v>551.30499999999995</v>
       </c>
     </row>
   </sheetData>
@@ -486,10 +469,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,79 +499,62 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D2">
         <v>4</v>
       </c>
       <c r="E2">
-        <v>31.081</v>
+        <v>29.98</v>
       </c>
       <c r="F2">
-        <v>88.281000000000006</v>
+        <v>73.037999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
         <v>9</v>
       </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
       <c r="C3">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D3">
         <v>3</v>
       </c>
       <c r="E3">
-        <v>26.574000000000002</v>
+        <v>25.937000000000001</v>
       </c>
       <c r="F3">
-        <v>65.807000000000002</v>
+        <v>70.295000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>23</v>
       </c>
       <c r="C4">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E4">
-        <v>32.561</v>
+        <v>23.638999999999999</v>
       </c>
       <c r="F4">
-        <v>83.266999999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>23</v>
-      </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>65.037000000000006</v>
-      </c>
-      <c r="F5">
-        <v>195.65700000000001</v>
+        <v>87.078000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>